<commit_message>
Draft update of KQ3 analysis
</commit_message>
<xml_diff>
--- a/data/KQ4 Workbook.xlsx
+++ b/data/KQ4 Workbook.xlsx
@@ -1,22 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27701"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fonnescj/Repositories/uterine_fibroids_MA/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="110" windowWidth="14340" windowHeight="6080"/>
+    <workbookView xWindow="400" yWindow="460" windowWidth="21640" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="98">
   <si>
     <t>Author</t>
   </si>
@@ -310,9 +323,6 @@
   </si>
   <si>
     <t>Median follow-up times by group</t>
-  </si>
-  <si>
-    <t>Morice</t>
   </si>
 </sst>
 </file>
@@ -429,12 +439,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -464,12 +474,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -673,28 +683,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N198"/>
+  <dimension ref="A1:N197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A194" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A198" sqref="A198:XFD198"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="1"/>
-    <col min="5" max="5" width="13.54296875" customWidth="1"/>
-    <col min="6" max="7" width="13.54296875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.26953125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="8.7265625" style="1"/>
-    <col min="13" max="13" width="11.36328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.36328125" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" style="1"/>
+    <col min="13" max="13" width="11.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -773,7 +783,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -805,7 +815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -837,7 +847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -869,7 +879,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -901,7 +911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -939,7 +949,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -984,7 +994,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1019,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -1051,7 +1061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1083,7 +1093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1147,7 +1157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -1275,7 +1285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1307,7 +1317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1339,7 +1349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1371,7 +1381,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1403,7 +1413,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1435,7 +1445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1467,7 +1477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1511,7 +1521,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1552,7 +1562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1594,7 +1604,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1676,7 +1686,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1717,7 +1727,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1799,7 +1809,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>
@@ -1837,7 +1847,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1875,7 +1885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>58</v>
       </c>
@@ -1913,7 +1923,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -1951,7 +1961,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -1989,7 +1999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>58</v>
       </c>
@@ -2027,7 +2037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2065,7 +2075,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -2103,7 +2113,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2141,7 +2151,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>58</v>
       </c>
@@ -2179,7 +2189,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2217,7 +2227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -2255,7 +2265,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2293,7 +2303,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -2369,7 +2379,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -2407,7 +2417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -2445,7 +2455,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -2486,7 +2496,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -2527,7 +2537,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -2568,7 +2578,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2609,7 +2619,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2650,7 +2660,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2691,7 +2701,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -2735,7 +2745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -2776,7 +2786,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -2817,7 +2827,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2855,7 +2865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>81</v>
       </c>
@@ -2899,7 +2909,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -2937,7 +2947,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>81</v>
       </c>
@@ -2975,7 +2985,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>81</v>
       </c>
@@ -3013,7 +3023,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -3092,7 +3102,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -3130,7 +3140,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -3168,7 +3178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -3209,7 +3219,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -3250,7 +3260,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -3291,7 +3301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -3332,7 +3342,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -3373,7 +3383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -3414,7 +3424,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -3455,7 +3465,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>81</v>
       </c>
@@ -3493,7 +3503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -3531,7 +3541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -3569,7 +3579,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -3607,7 +3617,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -3645,7 +3655,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -3683,7 +3693,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -3721,7 +3731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -3759,7 +3769,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -3797,7 +3807,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -3835,7 +3845,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -3873,7 +3883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -3911,7 +3921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>81</v>
       </c>
@@ -3949,7 +3959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -3987,7 +3997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>81</v>
       </c>
@@ -4025,7 +4035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>81</v>
       </c>
@@ -4063,7 +4073,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>81</v>
       </c>
@@ -4101,7 +4111,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>81</v>
       </c>
@@ -4139,7 +4149,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>81</v>
       </c>
@@ -4180,7 +4190,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -4221,7 +4231,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>72</v>
       </c>
@@ -4259,7 +4269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>72</v>
       </c>
@@ -4297,7 +4307,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>72</v>
       </c>
@@ -4335,7 +4345,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>72</v>
       </c>
@@ -4373,7 +4383,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>72</v>
       </c>
@@ -4411,7 +4421,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>72</v>
       </c>
@@ -4449,7 +4459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>84</v>
       </c>
@@ -4490,7 +4500,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>86</v>
       </c>
@@ -4531,7 +4541,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>86</v>
       </c>
@@ -4569,7 +4579,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>87</v>
       </c>
@@ -4610,7 +4620,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>87</v>
       </c>
@@ -4648,11 +4658,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>88</v>
       </c>
-      <c r="B105" s="1"/>
+      <c r="B105" s="1">
+        <v>364</v>
+      </c>
       <c r="C105" s="1">
         <v>37</v>
       </c>
@@ -4690,11 +4702,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>88</v>
       </c>
-      <c r="B106" s="1"/>
+      <c r="B106" s="1">
+        <v>364</v>
+      </c>
       <c r="D106" s="1" t="s">
         <v>36</v>
       </c>
@@ -4729,11 +4743,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>88</v>
       </c>
-      <c r="B107" s="1"/>
+      <c r="B107" s="1">
+        <v>364</v>
+      </c>
       <c r="D107" s="1" t="s">
         <v>36</v>
       </c>
@@ -4768,11 +4784,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>88</v>
       </c>
-      <c r="B108" s="1"/>
+      <c r="B108" s="1">
+        <v>364</v>
+      </c>
       <c r="D108" s="1" t="s">
         <v>36</v>
       </c>
@@ -4804,11 +4822,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>88</v>
       </c>
-      <c r="B109" s="1"/>
+      <c r="B109" s="1">
+        <v>364</v>
+      </c>
       <c r="D109" s="1" t="s">
         <v>36</v>
       </c>
@@ -4840,11 +4860,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>88</v>
       </c>
-      <c r="B110" s="1"/>
+      <c r="B110" s="1">
+        <v>364</v>
+      </c>
       <c r="D110" s="1" t="s">
         <v>36</v>
       </c>
@@ -4876,11 +4898,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>88</v>
       </c>
-      <c r="B111" s="1"/>
+      <c r="B111" s="1">
+        <v>364</v>
+      </c>
       <c r="D111" s="1" t="s">
         <v>36</v>
       </c>
@@ -4912,11 +4936,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>88</v>
       </c>
-      <c r="B112" s="1"/>
+      <c r="B112" s="1">
+        <v>364</v>
+      </c>
       <c r="D112" s="1" t="s">
         <v>36</v>
       </c>
@@ -4948,11 +4974,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>88</v>
       </c>
-      <c r="B113" s="1"/>
+      <c r="B113" s="1">
+        <v>364</v>
+      </c>
       <c r="D113" s="1" t="s">
         <v>36</v>
       </c>
@@ -4984,11 +5012,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>88</v>
       </c>
-      <c r="B114" s="1"/>
+      <c r="B114" s="1">
+        <v>364</v>
+      </c>
       <c r="D114" s="1" t="s">
         <v>36</v>
       </c>
@@ -5020,11 +5050,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>88</v>
       </c>
-      <c r="B115" s="1"/>
+      <c r="B115" s="1">
+        <v>364</v>
+      </c>
       <c r="D115" s="1" t="s">
         <v>36</v>
       </c>
@@ -5056,11 +5088,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>88</v>
       </c>
-      <c r="B116" s="1"/>
+      <c r="B116" s="1">
+        <v>364</v>
+      </c>
       <c r="D116" s="1" t="s">
         <v>36</v>
       </c>
@@ -5092,11 +5126,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>88</v>
       </c>
-      <c r="B117" s="1"/>
+      <c r="B117" s="1">
+        <v>364</v>
+      </c>
       <c r="D117" s="1" t="s">
         <v>36</v>
       </c>
@@ -5128,11 +5164,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>88</v>
       </c>
-      <c r="B118" s="1"/>
+      <c r="B118" s="1">
+        <v>364</v>
+      </c>
       <c r="D118" s="1" t="s">
         <v>36</v>
       </c>
@@ -5164,11 +5202,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>88</v>
       </c>
-      <c r="B119" s="1"/>
+      <c r="B119" s="1">
+        <v>364</v>
+      </c>
       <c r="D119" s="1" t="s">
         <v>36</v>
       </c>
@@ -5200,11 +5240,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>88</v>
       </c>
-      <c r="B120" s="1"/>
+      <c r="B120" s="1">
+        <v>364</v>
+      </c>
       <c r="D120" s="1" t="s">
         <v>36</v>
       </c>
@@ -5236,11 +5278,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>88</v>
       </c>
-      <c r="B121" s="1"/>
+      <c r="B121" s="1">
+        <v>364</v>
+      </c>
       <c r="D121" s="1" t="s">
         <v>36</v>
       </c>
@@ -5272,10 +5316,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>88</v>
       </c>
+      <c r="B122" s="1">
+        <v>364</v>
+      </c>
       <c r="D122" s="1" t="s">
         <v>36</v>
       </c>
@@ -5307,10 +5354,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>88</v>
       </c>
+      <c r="B123" s="1">
+        <v>364</v>
+      </c>
       <c r="D123" s="1" t="s">
         <v>36</v>
       </c>
@@ -5342,10 +5392,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>88</v>
       </c>
+      <c r="B124" s="1">
+        <v>364</v>
+      </c>
       <c r="D124" s="1" t="s">
         <v>36</v>
       </c>
@@ -5377,10 +5430,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>88</v>
       </c>
+      <c r="B125" s="1">
+        <v>364</v>
+      </c>
       <c r="D125" s="1" t="s">
         <v>36</v>
       </c>
@@ -5412,10 +5468,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>88</v>
       </c>
+      <c r="B126" s="1">
+        <v>364</v>
+      </c>
       <c r="D126" s="1" t="s">
         <v>36</v>
       </c>
@@ -5450,10 +5509,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>88</v>
       </c>
+      <c r="B127" s="1">
+        <v>364</v>
+      </c>
       <c r="D127" s="1" t="s">
         <v>36</v>
       </c>
@@ -5488,10 +5550,13 @@
         <v>94</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>88</v>
       </c>
+      <c r="B128" s="1">
+        <v>364</v>
+      </c>
       <c r="D128" s="1" t="s">
         <v>36</v>
       </c>
@@ -5526,10 +5591,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>88</v>
       </c>
+      <c r="B129" s="1">
+        <v>364</v>
+      </c>
       <c r="D129" s="1" t="s">
         <v>36</v>
       </c>
@@ -5561,10 +5629,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>88</v>
       </c>
+      <c r="B130" s="1">
+        <v>364</v>
+      </c>
       <c r="D130" s="1" t="s">
         <v>36</v>
       </c>
@@ -5596,10 +5667,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>88</v>
       </c>
+      <c r="B131" s="1">
+        <v>364</v>
+      </c>
       <c r="D131" s="1" t="s">
         <v>36</v>
       </c>
@@ -5631,10 +5705,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>88</v>
       </c>
+      <c r="B132" s="1">
+        <v>364</v>
+      </c>
       <c r="D132" s="1" t="s">
         <v>36</v>
       </c>
@@ -5666,10 +5743,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>88</v>
       </c>
+      <c r="B133" s="1">
+        <v>364</v>
+      </c>
       <c r="D133" s="1" t="s">
         <v>36</v>
       </c>
@@ -5701,10 +5781,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>88</v>
       </c>
+      <c r="B134" s="1">
+        <v>364</v>
+      </c>
       <c r="D134" s="1" t="s">
         <v>36</v>
       </c>
@@ -5736,10 +5819,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>88</v>
       </c>
+      <c r="B135" s="1">
+        <v>364</v>
+      </c>
       <c r="D135" s="1" t="s">
         <v>36</v>
       </c>
@@ -5771,10 +5857,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>88</v>
       </c>
+      <c r="B136" s="1">
+        <v>364</v>
+      </c>
       <c r="D136" s="1" t="s">
         <v>36</v>
       </c>
@@ -5806,10 +5895,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>88</v>
       </c>
+      <c r="B137" s="1">
+        <v>364</v>
+      </c>
       <c r="D137" s="1" t="s">
         <v>36</v>
       </c>
@@ -5841,10 +5933,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>88</v>
       </c>
+      <c r="B138" s="1">
+        <v>364</v>
+      </c>
       <c r="D138" s="1" t="s">
         <v>36</v>
       </c>
@@ -5876,10 +5971,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>88</v>
       </c>
+      <c r="B139" s="1">
+        <v>364</v>
+      </c>
       <c r="D139" s="1" t="s">
         <v>36</v>
       </c>
@@ -5911,10 +6009,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>88</v>
       </c>
+      <c r="B140" s="1">
+        <v>364</v>
+      </c>
       <c r="D140" s="1" t="s">
         <v>36</v>
       </c>
@@ -5946,10 +6047,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>88</v>
       </c>
+      <c r="B141" s="1">
+        <v>364</v>
+      </c>
       <c r="D141" s="1" t="s">
         <v>36</v>
       </c>
@@ -5981,10 +6085,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>51</v>
       </c>
+      <c r="B142">
+        <v>286</v>
+      </c>
       <c r="C142" s="1">
         <v>56</v>
       </c>
@@ -6022,10 +6129,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>51</v>
       </c>
+      <c r="B143">
+        <v>286</v>
+      </c>
       <c r="D143" s="1" t="s">
         <v>47</v>
       </c>
@@ -6057,10 +6167,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>51</v>
       </c>
+      <c r="B144">
+        <v>286</v>
+      </c>
       <c r="D144" s="1" t="s">
         <v>47</v>
       </c>
@@ -6092,10 +6205,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>51</v>
       </c>
+      <c r="B145">
+        <v>286</v>
+      </c>
       <c r="D145" s="1" t="s">
         <v>47</v>
       </c>
@@ -6127,10 +6243,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>51</v>
       </c>
+      <c r="B146">
+        <v>286</v>
+      </c>
       <c r="D146" s="1" t="s">
         <v>47</v>
       </c>
@@ -6162,10 +6281,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>51</v>
       </c>
+      <c r="B147">
+        <v>286</v>
+      </c>
       <c r="D147" s="1" t="s">
         <v>47</v>
       </c>
@@ -6197,10 +6319,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>51</v>
       </c>
+      <c r="B148">
+        <v>286</v>
+      </c>
       <c r="D148" s="1" t="s">
         <v>47</v>
       </c>
@@ -6232,10 +6357,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>51</v>
       </c>
+      <c r="B149">
+        <v>286</v>
+      </c>
       <c r="D149" s="1" t="s">
         <v>47</v>
       </c>
@@ -6267,10 +6395,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>51</v>
       </c>
+      <c r="B150">
+        <v>286</v>
+      </c>
       <c r="D150" s="1" t="s">
         <v>47</v>
       </c>
@@ -6302,10 +6433,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>51</v>
       </c>
+      <c r="B151">
+        <v>286</v>
+      </c>
       <c r="D151" s="1" t="s">
         <v>47</v>
       </c>
@@ -6337,10 +6471,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>51</v>
       </c>
+      <c r="B152">
+        <v>286</v>
+      </c>
       <c r="D152" s="1" t="s">
         <v>47</v>
       </c>
@@ -6372,10 +6509,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>51</v>
       </c>
+      <c r="B153">
+        <v>286</v>
+      </c>
       <c r="D153" s="1" t="s">
         <v>47</v>
       </c>
@@ -6407,10 +6547,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>51</v>
       </c>
+      <c r="B154">
+        <v>286</v>
+      </c>
       <c r="D154" s="1" t="s">
         <v>47</v>
       </c>
@@ -6442,10 +6585,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>51</v>
       </c>
+      <c r="B155">
+        <v>286</v>
+      </c>
       <c r="D155" s="1" t="s">
         <v>47</v>
       </c>
@@ -6477,10 +6623,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>51</v>
       </c>
+      <c r="B156">
+        <v>286</v>
+      </c>
       <c r="D156" s="1" t="s">
         <v>47</v>
       </c>
@@ -6512,10 +6661,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>51</v>
       </c>
+      <c r="B157">
+        <v>286</v>
+      </c>
       <c r="D157" s="1" t="s">
         <v>47</v>
       </c>
@@ -6547,10 +6699,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>51</v>
       </c>
+      <c r="B158">
+        <v>286</v>
+      </c>
       <c r="D158" s="1" t="s">
         <v>47</v>
       </c>
@@ -6582,10 +6737,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>51</v>
       </c>
+      <c r="B159">
+        <v>286</v>
+      </c>
       <c r="D159" s="1" t="s">
         <v>47</v>
       </c>
@@ -6617,10 +6775,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>51</v>
       </c>
+      <c r="B160">
+        <v>286</v>
+      </c>
       <c r="D160" s="1" t="s">
         <v>47</v>
       </c>
@@ -6652,10 +6813,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>51</v>
       </c>
+      <c r="B161">
+        <v>286</v>
+      </c>
       <c r="D161" s="1" t="s">
         <v>47</v>
       </c>
@@ -6687,10 +6851,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>51</v>
       </c>
+      <c r="B162">
+        <v>286</v>
+      </c>
       <c r="D162" s="1" t="s">
         <v>47</v>
       </c>
@@ -6722,10 +6889,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>51</v>
       </c>
+      <c r="B163">
+        <v>286</v>
+      </c>
       <c r="D163" s="1" t="s">
         <v>47</v>
       </c>
@@ -6757,10 +6927,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>51</v>
       </c>
+      <c r="B164">
+        <v>286</v>
+      </c>
       <c r="D164" s="1" t="s">
         <v>47</v>
       </c>
@@ -6792,10 +6965,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>51</v>
       </c>
+      <c r="B165">
+        <v>286</v>
+      </c>
       <c r="D165" s="1" t="s">
         <v>47</v>
       </c>
@@ -6827,10 +7003,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>51</v>
       </c>
+      <c r="B166">
+        <v>286</v>
+      </c>
       <c r="D166" s="1" t="s">
         <v>47</v>
       </c>
@@ -6862,10 +7041,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>51</v>
       </c>
+      <c r="B167">
+        <v>286</v>
+      </c>
       <c r="D167" s="1" t="s">
         <v>47</v>
       </c>
@@ -6897,10 +7079,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>51</v>
       </c>
+      <c r="B168">
+        <v>286</v>
+      </c>
       <c r="D168" s="1" t="s">
         <v>47</v>
       </c>
@@ -6932,10 +7117,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>51</v>
       </c>
+      <c r="B169">
+        <v>286</v>
+      </c>
       <c r="D169" s="1" t="s">
         <v>47</v>
       </c>
@@ -6967,10 +7155,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>51</v>
       </c>
+      <c r="B170">
+        <v>286</v>
+      </c>
       <c r="D170" s="1" t="s">
         <v>47</v>
       </c>
@@ -7002,10 +7193,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>51</v>
       </c>
+      <c r="B171">
+        <v>286</v>
+      </c>
       <c r="D171" s="1" t="s">
         <v>47</v>
       </c>
@@ -7037,10 +7231,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>51</v>
       </c>
+      <c r="B172">
+        <v>286</v>
+      </c>
       <c r="D172" s="1" t="s">
         <v>47</v>
       </c>
@@ -7072,10 +7269,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>51</v>
       </c>
+      <c r="B173">
+        <v>286</v>
+      </c>
       <c r="D173" s="1" t="s">
         <v>47</v>
       </c>
@@ -7107,10 +7307,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>51</v>
       </c>
+      <c r="B174">
+        <v>286</v>
+      </c>
       <c r="D174" s="1" t="s">
         <v>47</v>
       </c>
@@ -7142,10 +7345,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>51</v>
       </c>
+      <c r="B175">
+        <v>286</v>
+      </c>
       <c r="D175" s="1" t="s">
         <v>47</v>
       </c>
@@ -7177,10 +7383,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>51</v>
       </c>
+      <c r="B176">
+        <v>286</v>
+      </c>
       <c r="D176" s="1" t="s">
         <v>47</v>
       </c>
@@ -7212,10 +7421,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>51</v>
       </c>
+      <c r="B177">
+        <v>286</v>
+      </c>
       <c r="D177" s="1" t="s">
         <v>47</v>
       </c>
@@ -7247,10 +7459,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>51</v>
       </c>
+      <c r="B178">
+        <v>286</v>
+      </c>
       <c r="D178" s="1" t="s">
         <v>47</v>
       </c>
@@ -7282,10 +7497,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>51</v>
       </c>
+      <c r="B179">
+        <v>286</v>
+      </c>
       <c r="D179" s="1" t="s">
         <v>47</v>
       </c>
@@ -7317,10 +7535,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>51</v>
       </c>
+      <c r="B180">
+        <v>286</v>
+      </c>
       <c r="D180" s="1" t="s">
         <v>47</v>
       </c>
@@ -7352,10 +7573,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>51</v>
       </c>
+      <c r="B181">
+        <v>286</v>
+      </c>
       <c r="D181" s="1" t="s">
         <v>47</v>
       </c>
@@ -7387,10 +7611,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>51</v>
       </c>
+      <c r="B182">
+        <v>286</v>
+      </c>
       <c r="D182" s="1" t="s">
         <v>47</v>
       </c>
@@ -7422,10 +7649,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>51</v>
       </c>
+      <c r="B183">
+        <v>286</v>
+      </c>
       <c r="D183" s="1" t="s">
         <v>47</v>
       </c>
@@ -7457,10 +7687,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>51</v>
       </c>
+      <c r="B184">
+        <v>286</v>
+      </c>
       <c r="D184" s="1" t="s">
         <v>47</v>
       </c>
@@ -7492,10 +7725,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>51</v>
       </c>
+      <c r="B185">
+        <v>286</v>
+      </c>
       <c r="D185" s="1" t="s">
         <v>47</v>
       </c>
@@ -7527,10 +7763,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>51</v>
       </c>
+      <c r="B186">
+        <v>286</v>
+      </c>
       <c r="D186" s="1" t="s">
         <v>47</v>
       </c>
@@ -7562,10 +7801,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>51</v>
       </c>
+      <c r="B187">
+        <v>286</v>
+      </c>
       <c r="D187" s="1" t="s">
         <v>47</v>
       </c>
@@ -7597,10 +7839,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>51</v>
       </c>
+      <c r="B188">
+        <v>286</v>
+      </c>
       <c r="D188" s="1" t="s">
         <v>47</v>
       </c>
@@ -7632,10 +7877,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>51</v>
       </c>
+      <c r="B189">
+        <v>286</v>
+      </c>
       <c r="D189" s="1" t="s">
         <v>47</v>
       </c>
@@ -7667,10 +7915,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>51</v>
       </c>
+      <c r="B190">
+        <v>286</v>
+      </c>
       <c r="D190" s="1" t="s">
         <v>47</v>
       </c>
@@ -7702,10 +7953,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>51</v>
       </c>
+      <c r="B191">
+        <v>286</v>
+      </c>
       <c r="D191" s="1" t="s">
         <v>47</v>
       </c>
@@ -7737,10 +7991,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>51</v>
       </c>
+      <c r="B192">
+        <v>286</v>
+      </c>
       <c r="D192" s="1" t="s">
         <v>47</v>
       </c>
@@ -7772,10 +8029,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>51</v>
       </c>
+      <c r="B193">
+        <v>286</v>
+      </c>
       <c r="D193" s="1" t="s">
         <v>47</v>
       </c>
@@ -7807,10 +8067,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>51</v>
       </c>
+      <c r="B194">
+        <v>286</v>
+      </c>
       <c r="D194" s="1" t="s">
         <v>47</v>
       </c>
@@ -7842,10 +8105,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>51</v>
       </c>
+      <c r="B195">
+        <v>286</v>
+      </c>
       <c r="D195" s="1" t="s">
         <v>47</v>
       </c>
@@ -7877,10 +8143,13 @@
         <v>52</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>51</v>
       </c>
+      <c r="B196">
+        <v>286</v>
+      </c>
       <c r="D196" s="1" t="s">
         <v>47</v>
       </c>
@@ -7912,10 +8181,13 @@
         <v>28</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>51</v>
       </c>
+      <c r="B197">
+        <v>286</v>
+      </c>
       <c r="D197" s="1" t="s">
         <v>47</v>
       </c>
@@ -7945,14 +8217,6 @@
       </c>
       <c r="M197" s="1" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>98</v>
-      </c>
-      <c r="C198" s="1">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -7966,7 +8230,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7978,7 +8242,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>